<commit_message>
fix: Fix the position of `SOI55`.
</commit_message>
<xml_diff>
--- a/src/data/bell_suite.xlsx
+++ b/src/data/bell_suite.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEEA1FA-4589-46AE-940F-A07E71F67B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" r:id="rId1"/>
+    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -27,28 +22,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>Name</t>
+    <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t>Category</t>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
-    <t>Slug</t>
+    <t xml:space="preserve">Slug</t>
   </si>
   <si>
-    <t>Width</t>
+    <t xml:space="preserve">Width</t>
   </si>
   <si>
-    <t>Icon</t>
+    <t xml:space="preserve">Icon</t>
   </si>
   <si>
-    <t>Yak Mee Tarik</t>
+    <t xml:space="preserve">Yak Mee Tarik</t>
   </si>
   <si>
-    <t>restaurant</t>
+    <t xml:space="preserve">restaurant</t>
   </si>
   <si>
-    <t>Meyam Sophia</t>
+    <t xml:space="preserve">Meyam Sophia</t>
   </si>
   <si>
     <r>
@@ -68,8 +63,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>诊所</t>
+      <t xml:space="preserve">诊所</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">daily_necessity</t>
   </si>
   <si>
     <r>
@@ -89,21 +87,21 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>泰餐</t>
+      <t xml:space="preserve">泰餐</t>
     </r>
   </si>
   <si>
-    <t>学生之家餐厅</t>
-  </si>
-  <si>
-    <t>daily_necessity</t>
+    <t xml:space="preserve">学生之家餐厅</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,15 +110,24 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,112 +139,130 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -290,26 +315,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16384" width="11.54296875" style="1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.75" customHeight="1">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -331,7 +358,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="35.75" customHeight="1">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -347,7 +374,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="35.75" customHeight="1">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -363,12 +390,12 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="35.75" customHeight="1">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -379,9 +406,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A5"/>
-      <c r="B5"/>
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -391,11 +416,11 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -403,9 +428,13 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A7"/>
-      <c r="B7"/>
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -415,23 +444,19 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="35.75" customHeight="1">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -443,9 +468,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -455,9 +480,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A11"/>
-      <c r="B11"/>
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -467,9 +490,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A12"/>
-      <c r="B12"/>
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -479,9 +500,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>6</v>
@@ -495,7 +516,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="35.75" customHeight="1">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -507,7 +528,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="35.75" customHeight="1">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -519,7 +540,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="35.75" customHeight="1">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -531,7 +552,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="35.75" customHeight="1">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -543,7 +564,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="35.75" customHeight="1">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -555,7 +576,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="35.75" customHeight="1">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -567,7 +588,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="35.75" customHeight="1">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -579,7 +600,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="35.75" customHeight="1">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -591,7 +612,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="35.75" customHeight="1">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -603,7 +624,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="35.75" customHeight="1">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -615,7 +636,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="35.75" customHeight="1">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -627,7 +648,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="35.75" customHeight="1">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -639,7 +660,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="35.75" customHeight="1">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -651,7 +672,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="35.75" customHeight="1">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -663,8 +684,8 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A28" s="3"/>
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -675,7 +696,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="35.75" customHeight="1">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -687,7 +708,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="35.75" customHeight="1">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -699,8 +720,8 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A31" s="3"/>
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -711,7 +732,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="35.75" customHeight="1">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -723,7 +744,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="35.75" customHeight="1">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -735,7 +756,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="35.75" customHeight="1">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -747,7 +768,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" ht="35.75" customHeight="1">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -759,7 +780,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" ht="35.75" customHeight="1">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -771,9 +792,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -783,7 +804,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="35.75" customHeight="1">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -795,7 +816,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="35.75" customHeight="1">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -807,7 +828,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="35.75" customHeight="1">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -819,9 +840,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -831,7 +852,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="35.75" customHeight="1">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -843,7 +864,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="35.75" customHeight="1">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -855,7 +876,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="35.75" customHeight="1">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -867,7 +888,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" ht="35.75" customHeight="1">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -879,7 +900,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" ht="35.75" customHeight="1">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -891,7 +912,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="35.75" customHeight="1">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -903,7 +924,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" ht="35.75" customHeight="1">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -915,7 +936,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" ht="35.75" customHeight="1">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -927,8 +948,8 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A50" s="3"/>
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -939,7 +960,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" ht="35.75" customHeight="1">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -951,7 +972,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" ht="35.75" customHeight="1">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -963,7 +984,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="35.75" customHeight="1">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -975,7 +996,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" ht="35.75" customHeight="1">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -987,8 +1008,8 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A55" s="3"/>
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -999,8 +1020,8 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A56" s="3"/>
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1011,7 +1032,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" ht="35.75" customHeight="1">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1023,7 +1044,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="35.75" customHeight="1">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1035,8 +1056,8 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A59" s="3"/>
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1047,8 +1068,8 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A60" s="3"/>
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1059,7 +1080,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" ht="35.75" customHeight="1">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1071,8 +1092,8 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A62" s="3"/>
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -1083,7 +1104,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" ht="35.75" customHeight="1">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1095,7 +1116,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" ht="35.75" customHeight="1">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1107,8 +1128,8 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A65" s="3"/>
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -1119,8 +1140,8 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A66" s="3"/>
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="4"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -1131,7 +1152,7 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" ht="35.75" customHeight="1">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1143,8 +1164,8 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A68" s="3"/>
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -1155,7 +1176,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" ht="35.75" customHeight="1">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1167,8 +1188,8 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A70" s="3"/>
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -1179,10 +1200,10 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -1191,8 +1212,8 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A72" s="3"/>
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="4"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -1203,11 +1224,11 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A73" s="3"/>
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="4"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="3"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -1215,10 +1236,10 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -1227,8 +1248,8 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A75" s="3"/>
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="4"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -1239,7 +1260,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" ht="35.75" customHeight="1">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1251,7 +1272,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" ht="35.75" customHeight="1">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1263,7 +1284,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" ht="35.75" customHeight="1">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1276,16 +1297,16 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
-  <dataConsolidate/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{FDBB1088-6898-4A82-8AEF-85357824D4DA}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B5 B7 B9:B1078" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
feat: Add `Show` column to bell suite.
</commit_message>
<xml_diff>
--- a/src/data/bell_suite.xlsx
+++ b/src/data/bell_suite.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
   </si>
   <si>
     <t xml:space="preserve">Yak Mee Tarik</t>
@@ -326,9 +329,9 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7:D7"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,7 +355,9 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -360,10 +365,10 @@
     </row>
     <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -376,10 +381,10 @@
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -392,10 +397,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -417,10 +422,10 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -430,10 +435,10 @@
     </row>
     <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -445,11 +450,11 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -502,10 +507,10 @@
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>

</xml_diff>

<commit_message>
feat: Set default value of `Show` to  `true`.
</commit_message>
<xml_diff>
--- a/src/data/bell_suite.xlsx
+++ b/src/data/bell_suite.xlsx
@@ -101,8 +101,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -182,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,6 +193,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,7 +336,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,7 +378,9 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -389,7 +396,9 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -405,7 +414,9 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -415,19 +426,23 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -443,19 +458,23 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -467,19 +486,23 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -489,7 +512,9 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -499,14 +524,16 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -515,7 +542,9 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -690,7 +719,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -726,7 +755,7 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -798,8 +827,8 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -846,8 +875,8 @@
       <c r="J40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -954,7 +983,7 @@
       <c r="J49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4"/>
+      <c r="A50" s="5"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1014,7 +1043,7 @@
       <c r="J54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4"/>
+      <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1026,7 +1055,7 @@
       <c r="J55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4"/>
+      <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1062,7 +1091,7 @@
       <c r="J58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4"/>
+      <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1074,7 +1103,7 @@
       <c r="J59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4"/>
+      <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1098,7 +1127,7 @@
       <c r="J61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4"/>
+      <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -1134,7 +1163,7 @@
       <c r="J64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4"/>
+      <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -1146,7 +1175,7 @@
       <c r="J65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4"/>
+      <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -1170,7 +1199,7 @@
       <c r="J67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -1194,7 +1223,7 @@
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4"/>
+      <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -1206,9 +1235,9 @@
       <c r="J70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -1218,7 +1247,7 @@
       <c r="J71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4"/>
+      <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -1230,10 +1259,10 @@
       <c r="J72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
+      <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="4"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -1242,9 +1271,9 @@
       <c r="J73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -1254,7 +1283,7 @@
       <c r="J74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4"/>
+      <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>

</xml_diff>

<commit_message>
feat: Add columns of `Description` and `Image` to store SEO information of each store.
</commit_message>
<xml_diff>
--- a/src/data/bell_suite.xlsx
+++ b/src/data/bell_suite.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E07C775-E309-465D-A2CF-88674D46EA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" r:id="rId1"/>
+    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,76 +20,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>Yak Mee Tarik</t>
-  </si>
-  <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>daily_necessity</t>
-  </si>
-  <si>
-    <t>Student Home 湘村小灶</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>student</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>soi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sunsuriaclinic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>meyam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yak</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Soi 55
-</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yak Mee Tarik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meyam Sophia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meyam</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="宋体"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="134"/>
+        <charset val="1"/>
       </rPr>
-      <t>泰式餐厅</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Sunsuria Medical Clinic
 </t>
     </r>
@@ -105,23 +78,54 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>诊所</t>
+      <t xml:space="preserve">诊所</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Meyam Sophia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">daily_necessity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunsuriaclinic</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Soi 55
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">泰式餐厅</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">soi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student Home 湘村小灶</t>
+  </si>
+  <si>
+    <t xml:space="preserve">student</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -130,21 +134,29 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <name val="宋体"/>
+      <name val="LXGW WenKai Mono"/>
       <family val="2"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,119 +168,146 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -321,26 +360,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16384" width="11.54296875" style="1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.25" customHeight="1">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -359,24 +400,29 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="35.25" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="3" t="b">
+      <c r="F2" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G2" s="2"/>
@@ -384,19 +430,20 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="35.25" customHeight="1">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="3" t="b">
+      <c r="F3" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G3" s="2"/>
@@ -404,19 +451,20 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="35.25" customHeight="1">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3" t="b">
+      <c r="F4" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
@@ -424,13 +472,14 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3" t="b">
+      <c r="F5" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G5" s="2"/>
@@ -438,13 +487,14 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3" t="b">
+      <c r="F6" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G6" s="2"/>
@@ -452,19 +502,20 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="35.25" customHeight="1">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3" t="b">
+      <c r="F7" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G7" s="2"/>
@@ -472,13 +523,14 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3" t="b">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G8" s="2"/>
@@ -486,13 +538,14 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="35.25" customHeight="1">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3" t="b">
+      <c r="F9" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G9" s="2"/>
@@ -500,13 +553,14 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3" t="b">
+      <c r="F10" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G10" s="2"/>
@@ -514,19 +568,20 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A11" s="5" t="s">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3" t="b">
+      <c r="F11" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G11" s="2"/>
@@ -534,13 +589,14 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="3" t="b">
+      <c r="F12" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G12" s="2"/>
@@ -548,9 +604,10 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="35.25" customHeight="1">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E13" s="2"/>
-      <c r="F13" s="3" t="b">
+      <c r="F13" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G13" s="2"/>
@@ -558,7 +615,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="35.25" customHeight="1">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -570,7 +627,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="35.25" customHeight="1">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -582,7 +639,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="35.25" customHeight="1">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -594,7 +651,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="35.25" customHeight="1">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -606,7 +663,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="35.25" customHeight="1">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -618,7 +675,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="35.25" customHeight="1">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -630,7 +687,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="35.25" customHeight="1">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -642,7 +699,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="35.25" customHeight="1">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -654,7 +711,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="35.25" customHeight="1">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -666,7 +723,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="35.25" customHeight="1">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -678,7 +735,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="35.25" customHeight="1">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -690,7 +747,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="35.25" customHeight="1">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -702,7 +759,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="35.25" customHeight="1">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -714,7 +771,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="35.25" customHeight="1">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -726,8 +783,8 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A28" s="5"/>
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -738,7 +795,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="35.25" customHeight="1">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -750,7 +807,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="35.25" customHeight="1">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -762,8 +819,8 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A31" s="5"/>
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -774,7 +831,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="35.25" customHeight="1">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -786,7 +843,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="35.25" customHeight="1">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -798,7 +855,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="35.25" customHeight="1">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -810,7 +867,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" ht="35.25" customHeight="1">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -822,7 +879,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" ht="35.25" customHeight="1">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -834,9 +891,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -846,7 +903,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="35.25" customHeight="1">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -858,7 +915,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="35.25" customHeight="1">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -870,7 +927,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="35.25" customHeight="1">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -882,9 +939,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -894,7 +951,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="35.25" customHeight="1">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -906,7 +963,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="35.25" customHeight="1">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -918,7 +975,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="35.25" customHeight="1">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -930,7 +987,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" ht="35.25" customHeight="1">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -942,7 +999,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" ht="35.25" customHeight="1">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -954,7 +1011,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="35.25" customHeight="1">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -966,7 +1023,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" ht="35.25" customHeight="1">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -978,7 +1035,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" ht="35.25" customHeight="1">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -990,8 +1047,8 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A50" s="5"/>
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1002,7 +1059,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" ht="35.25" customHeight="1">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1014,7 +1071,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" ht="35.25" customHeight="1">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1026,7 +1083,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="35.25" customHeight="1">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1038,7 +1095,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" ht="35.25" customHeight="1">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1050,8 +1107,8 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A55" s="5"/>
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1062,8 +1119,8 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A56" s="5"/>
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1074,7 +1131,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" ht="35.25" customHeight="1">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1086,7 +1143,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="35.25" customHeight="1">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1098,8 +1155,8 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A59" s="5"/>
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1110,8 +1167,8 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A60" s="5"/>
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1122,7 +1179,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" ht="35.25" customHeight="1">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1134,8 +1191,8 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A62" s="5"/>
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -1146,7 +1203,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" ht="35.25" customHeight="1">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1158,7 +1215,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" ht="35.25" customHeight="1">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1170,8 +1227,8 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A65" s="5"/>
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -1182,8 +1239,8 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A66" s="5"/>
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -1194,7 +1251,7 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" ht="35.25" customHeight="1">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1206,8 +1263,8 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A68" s="5"/>
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -1218,7 +1275,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" ht="35.25" customHeight="1">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1230,8 +1287,8 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A70" s="5"/>
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -1242,10 +1299,10 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -1254,8 +1311,8 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A72" s="5"/>
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -1266,11 +1323,11 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A73" s="5"/>
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="8"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -1278,10 +1335,10 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -1290,8 +1347,8 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A75" s="5"/>
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -1302,7 +1359,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" ht="35.25" customHeight="1">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1314,7 +1371,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" ht="35.25" customHeight="1">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1326,7 +1383,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" ht="35.25" customHeight="1">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1339,16 +1396,16 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 B7 B14:B1078 B9:B12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B5 B7 B9:B12 B14:B1078" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
docs:Change name of YAK
</commit_message>
<xml_diff>
--- a/src/data/bell_suite.xlsx
+++ b/src/data/bell_suite.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DE22F6-CAC6-4844-B90F-AAD7CF56F157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="5410" yWindow="3450" windowWidth="19200" windowHeight="10790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="G" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -22,43 +38,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yak Mee Tarik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restaurant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meyam Sophia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meyam</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>yak</t>
+  </si>
+  <si>
+    <t>Meyam Sophia</t>
+  </si>
+  <si>
+    <t>meyam</t>
   </si>
   <si>
     <r>
@@ -78,14 +91,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">诊所</t>
+      <t>诊所</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">daily_necessity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sunsuriaclinic</t>
+    <t>daily_necessity</t>
+  </si>
+  <si>
+    <t>sunsuriaclinic</t>
   </si>
   <si>
     <r>
@@ -104,48 +117,36 @@
         <rFont val="LXGW WenKai Mono"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">泰式餐厅</t>
+      <t>泰式餐厅</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">soi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student Home 湘村小灶</t>
-  </si>
-  <si>
-    <t xml:space="preserve">student</t>
+    <t>soi</t>
+  </si>
+  <si>
+    <t>Student Home 湘村小灶</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>YAKMEETARIK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -158,6 +159,12 @@
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -168,146 +175,120 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -360,28 +341,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.54"/>
+    <col min="1" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="35.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -409,20 +388,20 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="35.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F2" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G2" s="2"/>
@@ -430,20 +409,20 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="35.25" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F3" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G3" s="2"/>
@@ -451,20 +430,20 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="35.25" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F4" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
@@ -472,14 +451,14 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="35.25" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F5" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G5" s="2"/>
@@ -487,14 +466,14 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="35.25" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F6" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G6" s="2"/>
@@ -502,20 +481,20 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="35.25" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F7" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G7" s="2"/>
@@ -523,14 +502,14 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="35.25" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F8" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G8" s="2"/>
@@ -538,14 +517,14 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="35.25" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F9" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G9" s="2"/>
@@ -553,14 +532,14 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="35.25" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F10" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G10" s="2"/>
@@ -568,20 +547,20 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="35.25" customHeight="1">
       <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F11" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G11" s="2"/>
@@ -589,14 +568,14 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" ht="35.25" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F12" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G12" s="2"/>
@@ -604,10 +583,10 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" ht="35.25" customHeight="1">
       <c r="E13" s="2"/>
-      <c r="F13" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F13" s="4" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G13" s="2"/>
@@ -615,7 +594,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" ht="35.25" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -627,7 +606,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" ht="35.25" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -639,7 +618,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" ht="35.25" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -651,7 +630,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" ht="35.25" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -663,7 +642,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="35.25" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -675,7 +654,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" ht="35.25" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -687,7 +666,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" ht="35.25" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -699,7 +678,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" ht="35.25" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -711,7 +690,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" ht="35.25" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -723,7 +702,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" ht="35.25" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -735,7 +714,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" ht="35.25" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -747,7 +726,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" ht="35.25" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -759,7 +738,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" ht="35.25" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -771,7 +750,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" ht="35.25" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -783,7 +762,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" ht="35.25" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -795,7 +774,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="35.25" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -807,7 +786,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" ht="35.25" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -819,7 +798,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" ht="35.25" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -831,7 +810,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" ht="35.25" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -843,7 +822,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="35.25" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -855,7 +834,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" ht="35.25" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -867,7 +846,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" ht="35.25" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -879,7 +858,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" ht="35.25" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -891,7 +870,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" ht="35.25" customHeight="1">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="2"/>
@@ -903,7 +882,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" ht="35.25" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -915,7 +894,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" ht="35.25" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -927,7 +906,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" ht="35.25" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -939,7 +918,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" ht="35.25" customHeight="1">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="2"/>
@@ -951,7 +930,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" ht="35.25" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -963,7 +942,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -975,7 +954,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" ht="35.25" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -987,7 +966,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" ht="35.25" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -999,7 +978,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:10" ht="35.25" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1011,7 +990,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:10" ht="35.25" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1023,7 +1002,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:10" ht="35.25" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1035,7 +1014,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:10" ht="35.25" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1047,7 +1026,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:10" ht="35.25" customHeight="1">
       <c r="A50" s="7"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1059,7 +1038,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:10" ht="35.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1071,7 +1050,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:10" ht="35.25" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1083,7 +1062,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:10" ht="35.25" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1095,7 +1074,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:10" ht="35.25" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1107,7 +1086,7 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:10" ht="35.25" customHeight="1">
       <c r="A55" s="7"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1119,7 +1098,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:10" ht="35.25" customHeight="1">
       <c r="A56" s="7"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1131,7 +1110,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:10" ht="35.25" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1143,7 +1122,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:10" ht="35.25" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1155,7 +1134,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:10" ht="35.25" customHeight="1">
       <c r="A59" s="7"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1167,7 +1146,7 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:10" ht="35.25" customHeight="1">
       <c r="A60" s="7"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1179,7 +1158,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:10" ht="35.25" customHeight="1">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1191,7 +1170,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:10" ht="35.25" customHeight="1">
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1203,7 +1182,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:10" ht="35.25" customHeight="1">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1215,7 +1194,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:10" ht="35.25" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1227,7 +1206,7 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:10" ht="35.25" customHeight="1">
       <c r="A65" s="7"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1239,7 +1218,7 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:10" ht="35.25" customHeight="1">
       <c r="A66" s="7"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1251,7 +1230,7 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:10" ht="35.25" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1263,7 +1242,7 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:10" ht="35.25" customHeight="1">
       <c r="A68" s="7"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1275,7 +1254,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:10" ht="35.25" customHeight="1">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1287,7 +1266,7 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:10" ht="35.25" customHeight="1">
       <c r="A70" s="7"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1299,7 +1278,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:10" ht="35.25" customHeight="1">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -1311,7 +1290,7 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:10" ht="35.25" customHeight="1">
       <c r="A72" s="7"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1323,7 +1302,7 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:10" ht="35.25" customHeight="1">
       <c r="A73" s="7"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1335,7 +1314,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:10" ht="35.25" customHeight="1">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -1347,7 +1326,7 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:10" ht="35.25" customHeight="1">
       <c r="A75" s="7"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -1359,7 +1338,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:10" ht="35.25" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1371,7 +1350,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:10" ht="35.25" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1383,7 +1362,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:10" ht="35.25" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1396,16 +1375,16 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B5 B7 B9:B12 B14:B1078" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 B7 B9:B12 B14:B1078" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>